<commit_message>
Aggiornamento preventivo (non completo)
</commit_message>
<xml_diff>
--- a/Preventivo/Costi,ricavi...xlsx
+++ b/Preventivo/Costi,ricavi...xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EBAC4862-A955-4FE5-B61C-A7F4930139BF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,94 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+  <si>
+    <t>Arduino Mega</t>
+  </si>
+  <si>
+    <t>Mosfet</t>
+  </si>
+  <si>
+    <t>Led blu 5 mm</t>
+  </si>
+  <si>
+    <t>Led verde 5mm</t>
+  </si>
+  <si>
+    <t>Led rosso 5 mm</t>
+  </si>
+  <si>
+    <t>Resistori 330 MΩ</t>
+  </si>
+  <si>
+    <t>Resistori 180 Ω</t>
+  </si>
+  <si>
+    <t>Resistori 390 Ω</t>
+  </si>
+  <si>
+    <t>Diodo</t>
+  </si>
+  <si>
+    <t>Morsetti elettrici</t>
+  </si>
+  <si>
+    <t>Pin M/F</t>
+  </si>
+  <si>
+    <t>Rame</t>
+  </si>
+  <si>
+    <t>pin jack</t>
+  </si>
+  <si>
+    <t>Alimentatore</t>
+  </si>
+  <si>
+    <t>Striscia led</t>
+  </si>
+  <si>
+    <t>Lastra multistrato 40*80 cm</t>
+  </si>
+  <si>
+    <t>APDS-9960</t>
+  </si>
+  <si>
+    <t>Nome componente</t>
+  </si>
+  <si>
+    <t>Quantitativo</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Resistore 1 KΩ</t>
+  </si>
+  <si>
+    <t>Prezzo (€)</t>
+  </si>
+  <si>
+    <t>Prezzo singolo (€)</t>
+  </si>
+  <si>
+    <t>Stoc</t>
+  </si>
+  <si>
+    <t>Per pezzo</t>
+  </si>
+  <si>
+    <t>Prezzo totale per pezzo (€)</t>
+  </si>
+  <si>
+    <t>Pezzi</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +136,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +427,547 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <f>G3*C3</f>
+        <v>8.73</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>8.73</v>
+      </c>
+      <c r="G3" s="4">
+        <f>F3/E3</f>
+        <v>8.73</v>
+      </c>
+      <c r="H3" s="4">
+        <f>SUM(D3:D20)</f>
+        <v>35.236433333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D20" si="0">G4*C4</f>
+        <v>1.4561999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3">
+        <v>24.27</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G20" si="1">F4/E4</f>
+        <v>0.4854</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="3">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>1.06E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>100</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.06</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>1.06E-2</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>100</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="E8" s="3">
+        <v>100</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>100</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>100</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>100</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="E12" s="3">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2.38</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2152</v>
+      </c>
+      <c r="E13" s="3">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3">
+        <v>5.38</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3800000000000001E-2</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4653333333333334</v>
+      </c>
+      <c r="E14" s="3">
+        <v>60</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2333333333333336E-2</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.34</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="1"/>
+        <v>2.34</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="1"/>
+        <v>3.3</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>1.944</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>6.48</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="1"/>
+        <v>1.296</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="1"/>
+        <v>3.9</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="0"/>
+        <v>3.12</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.56</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="1"/>
+        <v>1.56</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunta programma e libreria per sensore gesti
</commit_message>
<xml_diff>
--- a/Preventivo/Costi,ricavi...xlsx
+++ b/Preventivo/Costi,ricavi...xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D987F6F3-83BB-442E-BBC0-ABFDF235733D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beth/Desktop/NTSound/Preventivo/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -133,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,16 +168,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -189,16 +196,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,41 +482,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -535,7 +542,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -564,7 +571,7 @@
         <v>66.79443333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -590,7 +597,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -616,7 +623,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -642,7 +649,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -668,7 +675,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -694,7 +701,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -720,7 +727,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -746,7 +753,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -772,7 +779,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -798,7 +805,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -824,7 +831,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -850,7 +857,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -876,7 +883,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -902,7 +909,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -928,7 +935,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -954,7 +961,7 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -980,7 +987,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1006,7 +1013,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>0.29500000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1056,7 +1063,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1081,7 +1088,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1106,11 +1113,11 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="4">
@@ -1131,14 +1138,14 @@
         <v>9.8849999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>1</v>
       </c>
       <c r="D26" s="4"/>
@@ -1146,27 +1153,29 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>25</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>26</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>4</v>
       </c>
       <c r="D28" s="4">
@@ -1184,7 +1193,7 @@
         <v>0.19750000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>27</v>
       </c>

</xml_diff>